<commit_message>
Added photo permissions to paper
</commit_message>
<xml_diff>
--- a/Final Documentation/Project Expenditures and Budget.xlsx
+++ b/Final Documentation/Project Expenditures and Budget.xlsx
@@ -205,18 +205,12 @@
     <t>Digikey</t>
   </si>
   <si>
-    <t>XB24-AUI-001-ND</t>
-  </si>
-  <si>
     <t>RF TXRX Module 802.15.14 U. FL ANT (XBEE)</t>
   </si>
   <si>
     <t>RF TXRX Module 802.15.14 WIRE ANT (XBEE)</t>
   </si>
   <si>
-    <t>XB24-AWI-001-ND</t>
-  </si>
-  <si>
     <t>IC REG LDO 3.3V 1A TO220-3</t>
   </si>
   <si>
@@ -224,6 +218,12 @@
   </si>
   <si>
     <t>Digikey Taxes and Shipping</t>
+  </si>
+  <si>
+    <t>602-1559-ND</t>
+  </si>
+  <si>
+    <t>602-1560-ND</t>
   </si>
 </sst>
 </file>
@@ -1134,8 +1134,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="AG18" sqref="AG18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AC10" sqref="AC10:AF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,17 +1762,17 @@
         <v>17</v>
       </c>
       <c r="AD10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AE10" s="22">
-        <v>19</v>
+        <v>18.190000000000001</v>
       </c>
       <c r="AF10">
         <v>1</v>
       </c>
       <c r="AG10" s="22">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>18.190000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
@@ -1812,17 +1812,17 @@
         <v>18</v>
       </c>
       <c r="AD11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AE11" s="22">
-        <v>19.29</v>
+        <v>18.190000000000001</v>
       </c>
       <c r="AF11">
         <v>1</v>
       </c>
       <c r="AG11" s="22">
         <f t="shared" si="2"/>
-        <v>19.29</v>
+        <v>18.190000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
@@ -1855,7 +1855,7 @@
         <v>19</v>
       </c>
       <c r="AD12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AE12" s="22">
         <v>1.99</v>
@@ -1898,7 +1898,7 @@
         <v>20</v>
       </c>
       <c r="AD13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AE13" s="39">
         <f>3.39+3.33</f>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="AG18" s="22">
         <f>SUM(AG3:AG17)</f>
-        <v>91.39</v>
+        <v>89.48</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
@@ -2078,16 +2078,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="22">
-        <v>19</v>
+        <v>18.190000000000001</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s">
         <v>60</v>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="H19" s="29">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18.190000000000001</v>
       </c>
       <c r="K19" s="32"/>
       <c r="AC19" s="32"/>
@@ -2107,16 +2107,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="22">
-        <v>19.29</v>
+        <v>18.190000000000001</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F20" t="s">
         <v>60</v>
@@ -2126,7 +2126,7 @@
       </c>
       <c r="H20" s="29">
         <f t="shared" si="0"/>
-        <v>19.29</v>
+        <v>18.190000000000001</v>
       </c>
       <c r="K20" s="32"/>
       <c r="AC20" s="32"/>
@@ -2136,7 +2136,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21" s="22">
         <v>1.99</v>
@@ -2145,7 +2145,7 @@
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
         <v>60</v>
@@ -2167,7 +2167,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" s="39">
         <f>3.39+3.33</f>
@@ -2188,7 +2188,7 @@
         <v>6.7200000000000006</v>
       </c>
       <c r="I22">
-        <v>166402619</v>
+        <v>57396497</v>
       </c>
       <c r="K22" s="32"/>
     </row>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="H25" s="22">
         <f>SUM(H3:H24)</f>
-        <v>164.27999999999997</v>
+        <v>162.37</v>
       </c>
       <c r="K25" s="32"/>
     </row>

</xml_diff>